<commit_message>
Mock Project submission by Jan
</commit_message>
<xml_diff>
--- a/SeleniumTeamMockProject/Testdata/TestData.xlsx
+++ b/SeleniumTeamMockProject/Testdata/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856161CD-7CB7-0F40-8210-3E6BF3444D8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="23" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
@@ -27,26 +28,28 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Testing</t>
+    <t>vuppal@gmail.com</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Testing1</t>
-  </si>
-  <si>
-    <t>Testing2</t>
+    <t>test123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,15 +93,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -126,7 +132,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -404,20 +410,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -425,31 +431,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B9812260-0BF8-9E43-87EE-D2711D915DE5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>